<commit_message>
Some bug fixes, cleanup, and some changes
</commit_message>
<xml_diff>
--- a/Sample Spreadsheets/Real spreadsheet.xlsx
+++ b/Sample Spreadsheets/Real spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Your name (including last initial):</t>
   </si>
   <si>
-    <t>Will you be attending Friday's practice?</t>
-  </si>
-  <si>
     <t>Will you be attending Saturday's practice?</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>3987 Nobel Drive</t>
   </si>
   <si>
-    <t>Jerry L</t>
-  </si>
-  <si>
     <t>Yes!</t>
   </si>
   <si>
@@ -194,6 +188,15 @@
   </si>
   <si>
     <t>Yes, and I can drive!</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Will you be going to Friday's practice?</t>
+  </si>
+  <si>
+    <t>Jerry Lin</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:E22"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -594,19 +597,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -614,19 +617,19 @@
         <v>42222.350269444447</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -634,16 +637,16 @@
         <v>42222.012549699073</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -652,19 +655,19 @@
         <v>42219.417838668982</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -672,19 +675,19 @@
         <v>42220.260810243053</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -692,19 +695,19 @@
         <v>42222.960619895835</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -712,19 +715,19 @@
         <v>42220.418171423611</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -732,19 +735,19 @@
         <v>42219.895321087963</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -752,22 +755,22 @@
         <v>42219.428087476852</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -775,19 +778,19 @@
         <v>42219.335453159722</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -795,19 +798,19 @@
         <v>42219.610179826384</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -815,19 +818,19 @@
         <v>42219.450885115744</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -835,19 +838,19 @@
         <v>42219.372906122684</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -855,22 +858,22 @@
         <v>42219.30539400463</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -878,20 +881,20 @@
         <v>42219.56673737269</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -899,19 +902,19 @@
         <v>42219.412918391201</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -919,19 +922,19 @@
         <v>42222.653546342597</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -939,19 +942,19 @@
         <v>42219.476369918979</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -959,15 +962,15 @@
         <v>42219.344730821758</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -975,28 +978,28 @@
         <v>42220.522508391208</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>

</xml_diff>

<commit_message>
Started major work on generate
</commit_message>
<xml_diff>
--- a/Sample Spreadsheets/Real spreadsheet.xlsx
+++ b/Sample Spreadsheets/Real spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>Timestamp</t>
   </si>
@@ -196,7 +196,10 @@
     <t>Will you be going to Friday's practice?</t>
   </si>
   <si>
-    <t>Jerry Lin</t>
+    <t>Jerry L</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -784,7 +787,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -824,7 +827,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>

</xml_diff>